<commit_message>
Bug fix in .CSV Conversion
Small bug fix that ignored main .XLSX files if the current fund's -institutional.xlsx file was present.
</commit_message>
<xml_diff>
--- a/assets/ChartBuilder/public/Data/Backups/Rational/HRS/hrs-institutional.xlsx
+++ b/assets/ChartBuilder/public/Data/Backups/Rational/HRS/hrs-institutional.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Marketing Team Files\Marketing Materials\AutoCharts&amp;Tables\Backup Files\Rational\HRS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Dropbox (Catalyst Funds)\Marketing Team Files\Marketing Materials\AutoCharts&amp;Tables\Backup Files\Rational\HRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46947088-6E52-4833-BEE5-AF4F8B2B3BBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D991FB-A8DD-48B6-8944-17B3BA2F20FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15816" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Institutional" sheetId="7" r:id="rId1"/>
@@ -5186,7 +5186,7 @@
             <c:numRef>
               <c:f>[3]Institutional!$P$2:$P$109</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>41030</c:v>
@@ -5831,19 +5831,19 @@
                   <c:v>17540.772969589394</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>17586.378979310324</c:v>
+                  <c:v>17582.870824716407</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>17667.276322615151</c:v>
+                  <c:v>17663.752030510102</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>17729.111789744304</c:v>
+                  <c:v>17725.575162616889</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>17775.207480397639</c:v>
+                  <c:v>17771.661658039691</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>17830.310623586873</c:v>
+                  <c:v>17826.753809179616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5885,7 +5885,7 @@
             <c:numRef>
               <c:f>[3]Institutional!$P$2:$P$109</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>41030</c:v>
@@ -6584,7 +6584,7 @@
             <c:numRef>
               <c:f>[3]Institutional!$P$2:$P$109</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>41030</c:v>
@@ -7250,6 +7250,2293 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C655-4419-B5BF-0D4B8C6B256B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="536349000"/>
+        <c:axId val="536340472"/>
+        <c:extLst/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="536349000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="yyyy" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Trade Gothic LT Std" panose="00000500000000000000"/>
+                <a:ea typeface="Roboto Condensed Light" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Roboto Condensed Light" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536340472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="1"/>
+        <c:majorTimeUnit val="years"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="536340472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30000"/>
+          <c:min val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Trade Gothic LT Std" panose="00000500000000000000"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536349000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5000"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5060618006585718E-2"/>
+          <c:y val="3.6707400100090257E-2"/>
+          <c:w val="0.86844932707024103"/>
+          <c:h val="0.82745461772889894"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[3]Institutional!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tactical Program Composite (Net)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[3]Institutional!$P$2:$P$109</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41060</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41090</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41213</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41305</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41394</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41455</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41486</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41517</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41547</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41578</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41608</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41639</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41670</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41698</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41729</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41759</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41790</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41820</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41851</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41882</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41912</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41943</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41973</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42035</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42063</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42094</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42124</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42155</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42185</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42216</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42247</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42277</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42308</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42338</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42369</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42400</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42429</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42460</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42490</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>43373</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>43404</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>43434</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>43465</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>43496</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>43524</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>43555</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43616</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>43646</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43677</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>43708</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>43738</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>43769</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>43799</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>43830</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>43890</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>43982</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44012</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>44074</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>44165</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>44196</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>44227</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>44255</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>44286</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[3]Institutional!$T$2:$T$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10061.9112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10083.04121352</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10092.115950612168</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10078.996199876372</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10118.30428505589</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10123.363437198417</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10161.832218259771</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10143.540920266903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10201.359103512425</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10292.151199533684</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10366.254688170327</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10404.609830516558</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10451.430574753882</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10519.364873489782</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10638.233696560217</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10652.063400365747</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10828.887652811818</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10962.082970941403</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11241.616086700409</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11412.488651218257</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11697.800867498712</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11958.661826843934</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12152.392148438807</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12315.234203227887</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12497.499669435658</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12726.203913386331</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12839.467128215469</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12987.121000189947</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12452.051614982121</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12643.813209852848</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12885.310042161036</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13103.071781873556</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>13371.684753401963</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13267.385612325428</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>13328.415586142124</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>13427.045861479577</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13534.462228371414</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13603.48798573611</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13595.325892944667</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13429.462917050743</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13512.725587136458</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13664.068113712387</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13862.197101361215</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>13855.266002810535</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13966.108130833019</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>14089.009882384349</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>14134.094714007981</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>14163.776312907397</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>14243.093460259679</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>14362.735445325859</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>14427.367754829826</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>14502.390067154942</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>14512.541740201948</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>14564.786890466676</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14698.782929858971</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>14813.433436711872</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14921.57150079987</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>15070.787215807868</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>15230.53756029543</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>15356.951022045881</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>15449.092728178157</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>15538.697466001591</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>15610.175474345198</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>15721.007720213051</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>15865.640991239012</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>15849.775350247774</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>15819.660777082303</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>15906.668911356257</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>16022.787594409159</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>15997.151134258103</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>16059.540023681709</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>16120.5662757717</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>16176.988257736903</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>16364.641321526651</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>16459.556241191505</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>16624.151803603421</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>16625.81421878378</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>16665.716172908862</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>16655.716743205117</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>16727.3363252009</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>16792.572936869183</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>16878.215058847218</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>16972.733063176762</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>16969.338516564127</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>17093.214687735046</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>17221.413797893059</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>17192.137394436642</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>17266.063585232718</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>17274.696617025333</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>17352.432751801945</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>17420.107239533972</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>17400.945121570487</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>17418.346066692055</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>17420.087901298724</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>17501.962314434826</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>17582.471341081226</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>17540.273409862632</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>17606.926448820112</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>17668.550691390981</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>17486.564619269655</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>17540.772969589394</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>17582.870824716407</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>17663.752030510102</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>17725.575162616889</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>17771.661658039691</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>17826.753809179616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6209-4B49-9E01-AABEF9D4000D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[3]Institutional!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Barclay CTA Index</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[3]Institutional!$P$2:$P$109</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41060</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41090</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41213</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41305</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41394</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41455</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41486</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41517</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41547</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41578</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41608</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41639</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41670</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41698</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41729</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41759</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41790</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41820</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41851</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41882</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41912</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41943</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41973</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42035</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42063</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42094</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42124</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42155</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42185</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42216</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42247</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42277</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42308</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42338</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42369</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42400</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42429</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42460</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42490</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>43373</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>43404</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>43434</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>43465</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>43496</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>43524</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>43555</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43616</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>43646</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43677</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>43708</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>43738</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>43769</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>43799</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>43830</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>43890</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>43982</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44012</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>44074</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>44165</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>44196</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>44227</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>44255</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>44286</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[3]Institutional!$U$2:$U$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10264.320312118196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10038.061277392108</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10248.449200309902</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10202.78386956434</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10115.479084410461</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9904.3495526936986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9862.0675984964146</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9910.6070905319793</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10049.643361353845</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9963.5381369761726</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10009.001832149666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10090.32590118285</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9930.5963525833813</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9809.997775173606</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9738.8545937538802</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9651.7616968282746</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9594.4185906630446</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9659.1914550262118</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9710.1437388224695</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9770.104689872529</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9670.1276216469123</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9773.3376941297738</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9684.5838668986507</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9691.9042634303823</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9770.7027614845993</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9830.7423162322466</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9826.3097511987944</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9981.1214423710189</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10207.322378711933</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10141.445645030488</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10432.262238339399</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10513.924645027411</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10836.134871641871</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10819.091539473924</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10883.929337326403</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10718.048195002788</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10693.02146120173</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10464.253943257017</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10559.446438586079</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10375.206206547964</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10435.259431503888</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10327.367312686538</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10488.05035831325</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10356.635228605188</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10466.157519759437</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10647.492832538928</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10446.222938541141</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10424.121629311119</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10326.560770398262</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10536.292523318818</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10574.264944357132</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10397.307515777988</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10349.427611291732</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10215.278439928496</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>10195.521571417787</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10229.686839451268</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>10129.607244663581</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10196.39304719537</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>10146.134526469114</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>10156.951078767399</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>10164.425265142234</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>10060.364222194197</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>10118.985492833221</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>10171.5542787581</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>10055.415606798329</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>10248.910569839214</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>10246.347405787488</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>10300.929129880991</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10563.564588829186</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>10171.824265371552</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>10117.14001471598</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>10140.440884722211</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>10092.496046746644</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>10079.618710550769</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>10085.736128754224</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>10161.137580051884</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10129.880648829094</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9966.2345855585845</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9953.8562119647777</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9974.2419100561783</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9916.3314902474995</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9942.875617167183</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>10108.743089282521</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>10221.617999016427</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>10190.972809613982</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10409.009214062133</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>10494.352324328425</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>10741.789929225914</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>10524.857394096041</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10423.325339679044</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>10460.785127907011</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>10489.899253982558</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>10536.706047119158</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>10437.764497170438</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>10612.671394508199</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>10626.509062835454</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>10617.753294434757</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10560.044510198148</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10755.173063127999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10774.5232429425</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10660.06600660066</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10606.424109326124</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10766.867926308008</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>11058.272338572784</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>11038.809379540005</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11275.502200732655</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>11305.946056674633</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6209-4B49-9E01-AABEF9D4000D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[3]Institutional!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S&amp;P 500 TR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[3]Institutional!$P$2:$P$109</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41060</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41090</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41213</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41305</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41394</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41455</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41486</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41517</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41547</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41578</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41608</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41639</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41670</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41698</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41729</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41759</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41790</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41820</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41851</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41882</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41912</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41943</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41973</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42035</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42063</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42094</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42124</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42155</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42185</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42216</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42247</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42277</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42308</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42338</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42369</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42400</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42429</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42460</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42490</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42551</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42582</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42613</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>42643</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>42704</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>42735</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>42766</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>42794</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>42825</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>42855</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>42886</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>42916</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>42947</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>42978</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43039</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43069</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43100</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>43131</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>43159</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>43251</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>43281</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>43312</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>43343</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>43373</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>43404</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>43434</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>43465</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>43496</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>43524</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>43555</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>43616</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>43646</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43677</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>43708</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>43738</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>43769</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>43799</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>43830</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>43890</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>43951</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>43982</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44012</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>44074</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>44165</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>44196</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>44227</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>44255</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>44286</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[3]Institutional!$V$2:$V$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9398.9865116625679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9786.2483543234703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9922.1667453279333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10145.647547838471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10407.837974348146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10215.656076375952</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10274.900431394954</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10368.548741005703</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10905.598198242953</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11053.646984789395</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11468.191867252901</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11689.147229053333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11962.557236422652</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11801.922646993071</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12402.480727989338</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12043.288537811233</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12420.945425640264</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12991.90202946072</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13387.816611603783</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13726.763875433679</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13252.146624603594</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13858.37659703075</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13974.836674367198</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14078.131339477197</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14408.632867161823</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14706.262264947714</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14503.440395459178</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15083.670748772474</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14872.154739134399</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15235.404194715622</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15645.146599763193</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15605.733164418616</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15137.243212360589</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16007.236836657812</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15754.071755636705</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15905.225592236551</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16109.744889087617</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15797.873661723432</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16128.871997416605</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15155.749310678893</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14780.742065562103</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>16027.564564340781</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>16075.216732493731</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15821.679045466215</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>15036.556789295446</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>15016.270462279854</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>16034.933883134199</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>16097.117685537096</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16386.177145175585</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>16428.654229906195</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>17034.345993657425</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>17058.275579402347</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>17061.463430790514</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>16750.254614104389</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>17370.602214107701</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>17713.937948679744</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>18049.904364458369</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>18766.632718119432</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>18788.492270495415</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>18981.460781147805</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>19248.577887075557</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>19368.722623808713</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>19766.997043992371</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>19827.524819700116</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>20236.522012734869</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>20708.738024856983</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>21343.86566311451</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>21581.174288529557</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>22816.777206448598</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>21975.846850651262</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>21417.351847711812</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>21499.53217245865</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>22017.288918697403</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>22152.793303028076</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>22977.204792541288</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>23725.894461418753</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>23860.943438408263</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>22230.046948356841</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>22683.053050815215</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>20635.003436255425</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>22288.587492030405</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>23004.239428339621</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>23451.242434028074</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>24400.766740359893</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>22850.146144355884</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>24460.549304054817</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>24812.123771435228</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>24419.065835341295</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>24875.963600533276</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>25414.751885800433</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>26337.282957001305</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>27132.217171340835</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>27121.577199824496</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>24888.963410090204</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>21814.83965521527</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>24611.37193531563</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>25783.549030810413</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>26296.33769696371</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>27779.061198466559</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>29775.815386144062</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>28644.417948017359</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>27882.687068915588</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>30934.8270694124</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>32124.226842536747</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>31799.894014291556</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>32676.760149373655</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>34107.857018655188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6209-4B49-9E01-AABEF9D4000D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7494,6 +9781,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9081,6 +11408,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1330" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1197" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1330" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1197" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1197" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1197" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1197" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1197" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1862" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1197" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1197" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -9197,6 +12040,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2965</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>7649</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{930D9E65-AC00-4A8E-B977-DFCE29081C82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13614,7 +16495,7 @@
             <v>44165</v>
           </cell>
           <cell r="T105">
-            <v>17586.378979310324</v>
+            <v>17582.870824716407</v>
           </cell>
           <cell r="U105">
             <v>10766.867926308008</v>
@@ -13628,7 +16509,7 @@
             <v>44196</v>
           </cell>
           <cell r="T106">
-            <v>17667.276322615151</v>
+            <v>17663.752030510102</v>
           </cell>
           <cell r="U106">
             <v>11058.272338572784</v>
@@ -13642,7 +16523,7 @@
             <v>44227</v>
           </cell>
           <cell r="T107">
-            <v>17729.111789744304</v>
+            <v>17725.575162616889</v>
           </cell>
           <cell r="U107">
             <v>11038.809379540005</v>
@@ -13656,7 +16537,7 @@
             <v>44255</v>
           </cell>
           <cell r="T108">
-            <v>17775.207480397639</v>
+            <v>17771.661658039691</v>
           </cell>
           <cell r="U108">
             <v>11275.502200732655</v>
@@ -13670,7 +16551,7 @@
             <v>44286</v>
           </cell>
           <cell r="T109">
-            <v>17830.310623586873</v>
+            <v>17826.753809179616</v>
           </cell>
           <cell r="U109">
             <v>11305.946056674633</v>
@@ -13987,31 +16868,31 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="10.8"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="1"/>
-    <col min="15" max="15" width="3.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="26" width="8.7109375" style="1"/>
-    <col min="27" max="27" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7109375" style="1"/>
+    <col min="12" max="12" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="1"/>
+    <col min="15" max="15" width="3.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="26" width="8.6640625" style="1"/>
+    <col min="27" max="27" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="33.75">
+    <row r="1" spans="1:27" ht="32.4">
       <c r="A1" s="31"/>
       <c r="B1" s="32" t="s">
         <v>16</v>
@@ -14068,7 +16949,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="23.25" thickBot="1">
+    <row r="2" spans="1:27" ht="22.2" thickBot="1">
       <c r="A2" s="27" t="s">
         <v>17</v>
       </c>
@@ -14082,7 +16963,7 @@
       </c>
       <c r="D2" s="29">
         <f>L27*100</f>
-        <v>1.9657720758851749</v>
+        <v>1.9454318061712605</v>
       </c>
       <c r="E2" s="29">
         <f>L28*100</f>
@@ -14090,19 +16971,19 @@
       </c>
       <c r="F2" s="29">
         <f>L29*100</f>
-        <v>2.3548831935432668</v>
+        <v>2.3344653034188978</v>
       </c>
       <c r="G2" s="29">
         <f>L30*100</f>
-        <v>3.6824904580594842</v>
+        <v>3.6755957585805854</v>
       </c>
       <c r="H2" s="29">
         <f>L31*100</f>
-        <v>4.8227832951297955</v>
+        <v>4.8186009233615046</v>
       </c>
       <c r="I2" s="30">
         <f>L32*100</f>
-        <v>6.7007210584686616</v>
+        <v>6.6983337662633868</v>
       </c>
       <c r="P2" s="4">
         <v>41030</v>
@@ -14118,7 +16999,7 @@
       </c>
       <c r="AA2" s="35"/>
     </row>
-    <row r="3" spans="1:27" ht="12" thickBot="1">
+    <row r="3" spans="1:27" ht="11.4" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -14348,7 +17229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="22.5">
+    <row r="7" spans="1:27" ht="21.6">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
         <v>17</v>
@@ -14403,7 +17284,7 @@
       </c>
       <c r="B8" s="20">
         <f>I2/100</f>
-        <v>6.7007210584686616E-2</v>
+        <v>6.6983337662633868E-2</v>
       </c>
       <c r="C8" s="38">
         <f>I3/100</f>
@@ -14457,7 +17338,7 @@
       </c>
       <c r="B9" s="23">
         <f>STDEV(Q3:Q109)*SQRT(12)</f>
-        <v>2.7374855857228174E-2</v>
+        <v>2.737729528184607E-2</v>
       </c>
       <c r="C9" s="23">
         <f>STDEV(R3:R109)*SQRT(12)</f>
@@ -14643,7 +17524,7 @@
       </c>
       <c r="G13" s="1">
         <f>VLOOKUP($K$21,$P:$V,5,0)</f>
-        <v>17830.310623586873</v>
+        <v>17826.753809179616</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>16</v>
@@ -14654,7 +17535,7 @@
       </c>
       <c r="L13" s="1">
         <f t="shared" ref="L13:L21" si="2">VLOOKUP($K13,$P:$V,5,0)</f>
-        <v>17775.207480397639</v>
+        <v>17771.661658039691</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" ref="M13:M21" si="3">VLOOKUP($K13,$P:$V,6,0)</f>
@@ -14719,7 +17600,7 @@
       </c>
       <c r="L14" s="1">
         <f t="shared" si="2"/>
-        <v>17667.276322615151</v>
+        <v>17663.752030510102</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" si="3"/>
@@ -14841,7 +17722,7 @@
       </c>
       <c r="L16" s="1">
         <f t="shared" si="2"/>
-        <v>17667.276322615151</v>
+        <v>17663.752030510102</v>
       </c>
       <c r="M16" s="1">
         <f t="shared" si="3"/>
@@ -15129,7 +18010,7 @@
       </c>
       <c r="L21" s="1">
         <f t="shared" si="2"/>
-        <v>17830.310623586873</v>
+        <v>17826.753809179616</v>
       </c>
       <c r="M21" s="1">
         <f t="shared" si="3"/>
@@ -15362,7 +18243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="22.5">
+    <row r="26" spans="1:25" ht="21.6">
       <c r="A26" s="16"/>
       <c r="B26" s="17" t="s">
         <v>17</v>
@@ -15433,7 +18314,7 @@
       </c>
       <c r="B27" s="19">
         <f>B8/B9</f>
-        <v>2.4477648735086852</v>
+        <v>2.4466747709387726</v>
       </c>
       <c r="C27" s="37">
         <f>C8/C9</f>
@@ -15448,7 +18329,7 @@
       </c>
       <c r="L27" s="26">
         <f t="shared" si="6"/>
-        <v>1.9657720758851749E-2</v>
+        <v>1.9454318061712605E-2</v>
       </c>
       <c r="M27" s="26">
         <f t="shared" si="6"/>
@@ -15588,7 +18469,7 @@
       </c>
       <c r="L29" s="26">
         <f t="shared" si="6"/>
-        <v>2.3548831935432668E-2</v>
+        <v>2.3344653034188978E-2</v>
       </c>
       <c r="M29" s="26">
         <f t="shared" si="6"/>
@@ -15643,7 +18524,7 @@
       </c>
       <c r="L30" s="26">
         <f>(L$21/L18)^(1/3)-1</f>
-        <v>3.6824904580594842E-2</v>
+        <v>3.6755957585805854E-2</v>
       </c>
       <c r="M30" s="26">
         <f>(M$21/M18)^(1/3)-1</f>
@@ -15692,7 +18573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="22.5">
+    <row r="31" spans="1:25" ht="21.6">
       <c r="A31" s="16"/>
       <c r="B31" s="17" t="s">
         <v>17</v>
@@ -15708,7 +18589,7 @@
       </c>
       <c r="L31" s="26">
         <f>(L$21/L19)^(1/5)-1</f>
-        <v>4.8227832951297955E-2</v>
+        <v>4.8186009233615046E-2</v>
       </c>
       <c r="M31" s="26">
         <f>(M$21/M19)^(1/5)-1</f>
@@ -15778,7 +18659,7 @@
       </c>
       <c r="L32" s="26">
         <f>(L$21/L20)^(12/(COUNTA($P:$P)-2))-1</f>
-        <v>6.7007210584686616E-2</v>
+        <v>6.6983337662633868E-2</v>
       </c>
       <c r="M32" s="26">
         <f>(M$21/M20)^(12/(COUNTA($P:$P)-2))-1</f>
@@ -16310,7 +19191,7 @@
       </c>
       <c r="B40" s="42">
         <f t="shared" si="7"/>
-        <v>1.4188723392026148E-2</v>
+        <v>1.3986411657856523E-2</v>
       </c>
       <c r="C40" s="42">
         <f t="shared" si="7"/>
@@ -16571,7 +19452,7 @@
       </c>
       <c r="L44" s="1">
         <f t="shared" si="8"/>
-        <v>17667.276322615151</v>
+        <v>17663.752030510102</v>
       </c>
       <c r="M44" s="1">
         <f t="shared" si="9"/>
@@ -16629,7 +19510,7 @@
       </c>
       <c r="L45" s="1">
         <f t="shared" si="8"/>
-        <v>17830.310623586873</v>
+        <v>17826.753809179616</v>
       </c>
       <c r="M45" s="1">
         <f t="shared" si="9"/>
@@ -17202,7 +20083,7 @@
       </c>
       <c r="L56" s="26">
         <f t="shared" si="12"/>
-        <v>1.4188723392026148E-2</v>
+        <v>1.3986411657856523E-2</v>
       </c>
       <c r="M56" s="26">
         <f t="shared" si="12"/>
@@ -19142,8 +22023,8 @@
         <f t="shared" si="15"/>
         <v>44165</v>
       </c>
-      <c r="Q105" s="9">
-        <v>2.5999999999999999E-3</v>
+      <c r="Q105" s="46">
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="R105" s="9">
         <v>1.5127041435275768E-2</v>
@@ -19153,7 +22034,7 @@
       </c>
       <c r="T105" s="1">
         <f t="shared" si="17"/>
-        <v>17586.378979310324</v>
+        <v>17582.870824716407</v>
       </c>
       <c r="U105" s="1">
         <f t="shared" si="17"/>
@@ -19165,7 +22046,7 @@
       </c>
       <c r="W105" s="26">
         <f>T105/MAX(T$2:T105)-1</f>
-        <v>-4.6507330179998974E-3</v>
+        <v>-4.8492866319999051E-3</v>
       </c>
       <c r="X105" s="26">
         <f>U105/MAX(U$2:U105)-1</f>
@@ -19192,7 +22073,7 @@
       </c>
       <c r="T106" s="1">
         <f t="shared" si="17"/>
-        <v>17667.276322615151</v>
+        <v>17663.752030510102</v>
       </c>
       <c r="U106" s="1">
         <f t="shared" si="17"/>
@@ -19204,7 +22085,7 @@
       </c>
       <c r="W106" s="26">
         <f>T106/MAX(T$2:T106)-1</f>
-        <v>-7.2126389882742892E-5</v>
+        <v>-2.7159335050708222E-4</v>
       </c>
       <c r="X106" s="26">
         <f>U106/MAX(U$2:U106)-1</f>
@@ -19231,7 +22112,7 @@
       </c>
       <c r="T107" s="1">
         <f t="shared" si="17"/>
-        <v>17729.111789744304</v>
+        <v>17725.575162616889</v>
       </c>
       <c r="U107" s="1">
         <f t="shared" si="17"/>
@@ -19270,7 +22151,7 @@
       </c>
       <c r="T108" s="1">
         <f t="shared" si="17"/>
-        <v>17775.207480397639</v>
+        <v>17771.661658039691</v>
       </c>
       <c r="U108" s="1">
         <f t="shared" si="17"/>
@@ -19309,7 +22190,7 @@
       </c>
       <c r="T109" s="1">
         <f t="shared" si="17"/>
-        <v>17830.310623586873</v>
+        <v>17826.753809179616</v>
       </c>
       <c r="U109" s="1">
         <f t="shared" si="17"/>
@@ -19358,12 +22239,12 @@
       <selection activeCell="A106" sqref="A106:D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -21241,7 +24122,7 @@
       </c>
       <c r="B105" s="50">
         <f>Institutional!T105</f>
-        <v>17586.378979310324</v>
+        <v>17582.870824716407</v>
       </c>
       <c r="C105" s="50">
         <f>Institutional!U105</f>
@@ -21259,7 +24140,7 @@
       </c>
       <c r="B106" s="50">
         <f>Institutional!T106</f>
-        <v>17667.276322615151</v>
+        <v>17663.752030510102</v>
       </c>
       <c r="C106" s="50">
         <f>Institutional!U106</f>
@@ -21277,7 +24158,7 @@
       </c>
       <c r="B107" s="50">
         <f>Institutional!T107</f>
-        <v>17729.111789744304</v>
+        <v>17725.575162616889</v>
       </c>
       <c r="C107" s="50">
         <f>Institutional!U107</f>
@@ -21295,7 +24176,7 @@
       </c>
       <c r="B108" s="50">
         <f>Institutional!T108</f>
-        <v>17775.207480397639</v>
+        <v>17771.661658039691</v>
       </c>
       <c r="C108" s="50">
         <f>Institutional!U108</f>
@@ -21313,7 +24194,7 @@
       </c>
       <c r="B109" s="50">
         <f>Institutional!T109</f>
-        <v>17830.310623586873</v>
+        <v>17826.753809179616</v>
       </c>
       <c r="C109" s="50">
         <f>Institutional!U109</f>
@@ -21340,11 +24221,11 @@
       <selection activeCell="A106" sqref="A106:D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="9.140625" style="50"/>
-    <col min="9" max="9" width="14.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="9.109375" style="50"/>
+    <col min="9" max="9" width="14.6640625" style="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -21394,7 +24275,7 @@
       </c>
       <c r="D2" s="50">
         <f>Institutional!D2</f>
-        <v>1.9657720758851749</v>
+        <v>1.9454318061712605</v>
       </c>
       <c r="E2" s="50">
         <f>Institutional!E2</f>
@@ -21402,19 +24283,19 @@
       </c>
       <c r="F2" s="50">
         <f>Institutional!F2</f>
-        <v>2.3548831935432668</v>
+        <v>2.3344653034188978</v>
       </c>
       <c r="G2" s="50">
         <f>Institutional!G2</f>
-        <v>3.6824904580594842</v>
+        <v>3.6755957585805854</v>
       </c>
       <c r="H2" s="50">
         <f>Institutional!H2</f>
-        <v>4.8227832951297955</v>
+        <v>4.8186009233615046</v>
       </c>
       <c r="I2" s="50">
         <f>Institutional!I2</f>
-        <v>6.7007210584686616</v>
+        <v>6.6983337662633868</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -21518,13 +24399,13 @@
       <selection activeCell="A106" sqref="A106:D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21719,7 +24600,7 @@
       </c>
       <c r="B10" s="50">
         <f>Institutional!L56*100</f>
-        <v>1.4188723392026148</v>
+        <v>1.3986411657856523</v>
       </c>
       <c r="C10" s="50">
         <f>Institutional!M56*100</f>
@@ -21771,9 +24652,9 @@
       <selection activeCell="A106" sqref="A106:D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21799,7 +24680,7 @@
       </c>
       <c r="B2" s="50">
         <f>Institutional!B27</f>
-        <v>2.4477648735086852</v>
+        <v>2.4466747709387726</v>
       </c>
       <c r="C2" s="50">
         <f>Institutional!C27</f>
@@ -21869,13 +24750,13 @@
       <selection activeCell="A106" sqref="A106:D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21902,11 +24783,11 @@
     <row r="2" spans="1:6">
       <c r="A2" s="50">
         <f>Institutional!B8*100</f>
-        <v>6.7007210584686616</v>
+        <v>6.6983337662633868</v>
       </c>
       <c r="B2" s="50">
         <f>Institutional!B9*100</f>
-        <v>2.7374855857228173</v>
+        <v>2.737729528184607</v>
       </c>
       <c r="C2" s="50">
         <f>Institutional!C8*100</f>

</xml_diff>